<commit_message>
user input settings file
</commit_message>
<xml_diff>
--- a/GENeSYS-MOD_User_Input_Settings_v02_phe_06-09-2023.xlsx
+++ b/GENeSYS-MOD_User_Input_Settings_v02_phe_06-09-2023.xlsx
@@ -8,18 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dozeumhep\Documents\git\GENeSYS-MOD_GroupRepo\GENeSYS-MOD_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D120BE0-4176-4E78-800F-0D8BA7FCDD40}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EF9D38-D2AA-4D71-9148-4A6B4F0C3100}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
     <sheet name="Technology_selection" sheetId="2" r:id="rId2"/>
-    <sheet name="Technology_in_region_selection" sheetId="3" r:id="rId3"/>
-    <sheet name="Year_selection" sheetId="4" r:id="rId4"/>
+    <sheet name="Year_selection" sheetId="4" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="Technologies">#REF!:B</definedName>
@@ -1775,7 +1774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
   <dimension ref="A1:B145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B139" sqref="B139"/>
     </sheetView>
   </sheetViews>
@@ -2952,22 +2951,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E64D1206-FE0C-4D30-B550-10017D0BE07E}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D817F8-1014-4E28-A827-54661E8BA006}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>